<commit_message>
second commit with some methods
</commit_message>
<xml_diff>
--- a/code_1/01.xlsx
+++ b/code_1/01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E_disk\C_documents\E_建模\B_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\研一下\数模\Code-For-training\code_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67DB268-EE4C-49B8-AAEF-23B6865F5567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490620BE-7655-4D7C-AE50-99589F1C92BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30869" yWindow="-109" windowWidth="23452" windowHeight="12827" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>